<commit_message>
Updated salary Excel file and env setup
</commit_message>
<xml_diff>
--- a/server/uploads/Book1.xlsx
+++ b/server/uploads/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\OneDrive\Desktop\projects\HRMS system\server\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F62A466-A236-4EAE-97A2-E43BDDC41140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24F9E37-01E6-4751-A767-C2F428F5C7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DCCC6805-F783-44CF-8F5A-645AFE77ABF3}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DCCC6805-F783-44CF-8F5A-645AFE77ABF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -935,9 +935,6 @@
     <t>₹35,056</t>
   </si>
   <si>
-    <t>6866356c0dd3398c963b6e67</t>
-  </si>
-  <si>
     <t>Anushka</t>
   </si>
   <si>
@@ -947,9 +944,6 @@
     <t>Anu</t>
   </si>
   <si>
-    <t>68666d8ccc22e35794181251</t>
-  </si>
-  <si>
     <t>Trisha</t>
   </si>
   <si>
@@ -963,6 +957,12 @@
   </si>
   <si>
     <t>687df249015240f72575d2ad</t>
+  </si>
+  <si>
+    <t>69067bfe21810f4deae03b5c</t>
+  </si>
+  <si>
+    <t>6907a4d6f37984871bfd0e75</t>
   </si>
 </sst>
 </file>
@@ -1039,12 +1039,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1387,7 +1386,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L38" sqref="A1:L38"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1396,10 +1395,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -1434,11 +1433,11 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1469,11 +1468,11 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>
@@ -1507,11 +1506,11 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -1542,11 +1541,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -1577,11 +1576,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C6" t="s">
         <v>49</v>
@@ -1615,11 +1614,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>300</v>
       </c>
       <c r="C7" t="s">
         <v>58</v>
@@ -1653,11 +1652,11 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -1688,11 +1687,11 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
@@ -1726,11 +1725,11 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1761,11 +1760,11 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
@@ -1799,11 +1798,11 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C12" t="s">
         <v>49</v>
@@ -1837,11 +1836,11 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>302</v>
       </c>
       <c r="C13" t="s">
         <v>58</v>
@@ -1872,11 +1871,11 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>304</v>
+      <c r="A14" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1910,11 +1909,11 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>304</v>
+      <c r="A15" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C15" t="s">
         <v>21</v>
@@ -1948,11 +1947,11 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>304</v>
+      <c r="A16" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
@@ -1983,11 +1982,11 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>304</v>
+      <c r="A17" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C17" t="s">
         <v>40</v>
@@ -2018,11 +2017,11 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>304</v>
+      <c r="A18" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C18" t="s">
         <v>49</v>
@@ -2053,11 +2052,11 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>304</v>
+      <c r="A19" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C19" t="s">
         <v>58</v>
@@ -2091,11 +2090,11 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>306</v>
+      <c r="A20" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -2129,11 +2128,11 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>306</v>
+      <c r="A21" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>
@@ -2167,11 +2166,11 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>306</v>
+      <c r="A22" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C22" t="s">
         <v>31</v>
@@ -2202,11 +2201,11 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>306</v>
+      <c r="A23" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C23" t="s">
         <v>40</v>
@@ -2240,11 +2239,11 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>306</v>
+      <c r="A24" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C24" t="s">
         <v>49</v>
@@ -2278,11 +2277,11 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>306</v>
+      <c r="A25" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="C25" t="s">
         <v>58</v>
@@ -2316,11 +2315,11 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>300</v>
+      <c r="A26" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
@@ -2354,11 +2353,11 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>300</v>
+      <c r="A27" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C27" t="s">
         <v>21</v>
@@ -2392,11 +2391,11 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>300</v>
+      <c r="A28" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C28" t="s">
         <v>31</v>
@@ -2427,11 +2426,11 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>300</v>
+      <c r="A29" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C29" t="s">
         <v>40</v>
@@ -2462,11 +2461,11 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>300</v>
+      <c r="A30" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C30" t="s">
         <v>49</v>
@@ -2500,11 +2499,11 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>300</v>
+      <c r="A31" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="C31" t="s">
         <v>58</v>
@@ -2535,16 +2534,16 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>304</v>
+      <c r="A32" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>28838</v>
       </c>
       <c r="E32" t="s">
@@ -2570,11 +2569,11 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>304</v>
+      <c r="A33" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C33" t="s">
         <v>21</v>
@@ -2605,11 +2604,11 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>304</v>
+      <c r="A34" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
@@ -2643,11 +2642,11 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>304</v>
+      <c r="A35" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C35" t="s">
         <v>40</v>
@@ -2681,11 +2680,11 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>304</v>
+      <c r="A36" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C36" t="s">
         <v>49</v>
@@ -2719,11 +2718,11 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>304</v>
+      <c r="A37" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>302</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
@@ -2754,8 +2753,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="4"/>
-      <c r="B38" s="2"/>
+      <c r="A38" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: remove temp excel and add correct salary sheet
</commit_message>
<xml_diff>
--- a/server/uploads/Book1.xlsx
+++ b/server/uploads/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anush\OneDrive\Desktop\projects\HRMS system\server\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24F9E37-01E6-4751-A767-C2F428F5C7CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5490D53F-7A9B-4E3B-A828-58861BCA5C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{DCCC6805-F783-44CF-8F5A-645AFE77ABF3}"/>
   </bookViews>
@@ -1386,7 +1386,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="I39" sqref="A1:I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>